<commit_message>
feito parcial, n deu muito certo
</commit_message>
<xml_diff>
--- a/Projecao_MegaSenaValor/Resultados_Passados.xlsx
+++ b/Projecao_MegaSenaValor/Resultados_Passados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14b3bf11c301978b/Documents/GitHub/Python_Tecnics/Projecao_MegaSenaValor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFC222C6-00C6-4505-8DE6-79044724D470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{DFC222C6-00C6-4505-8DE6-79044724D470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{255FC7EE-F42E-495F-A1AF-5608FC0918F8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A8E69F22-01A5-4FB6-8ECB-7CE192C04F54}"/>
   </bookViews>
@@ -8867,11 +8867,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61E3042-6D75-4080-9C08-C68E3F288624}">
   <dimension ref="A1:H2810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>